<commit_message>
Agregada la tabla MISMOS
</commit_message>
<xml_diff>
--- a/assets/casos-de-uso.xlsx
+++ b/assets/casos-de-uso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ldlc\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB8DF50-813E-4FCD-A0DA-0DB1F88ED53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A21D96B-70D7-4AEF-B094-FF95F7973C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BD85DA4A-5FD3-4E65-8B17-D09145574319}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="148">
   <si>
     <t>mercadona</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>MARCAS_BLANCAS</t>
+  </si>
+  <si>
+    <t>MISMOS</t>
   </si>
 </sst>
 </file>
@@ -646,7 +649,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -923,6 +926,9 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -940,6 +946,15 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2773,8 +2788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C2794B-2B9E-4E07-929E-524469B5B597}">
   <dimension ref="A2:S92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K72" sqref="K72"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4196,10 +4211,10 @@
       </c>
       <c r="K37" s="51"/>
       <c r="M37" s="44"/>
-      <c r="N37" s="96" t="s">
+      <c r="N37" s="97" t="s">
         <v>146</v>
       </c>
-      <c r="O37" s="97"/>
+      <c r="O37" s="98"/>
       <c r="P37" s="28"/>
       <c r="Q37" s="40" t="s">
         <v>109</v>
@@ -4213,7 +4228,7 @@
       <c r="A38" s="95" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="100" t="s">
+      <c r="B38" s="101" t="s">
         <v>142</v>
       </c>
       <c r="C38" s="79" t="s">
@@ -4231,7 +4246,7 @@
       <c r="G38" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="H38" s="101" t="s">
+      <c r="H38" s="102" t="s">
         <v>144</v>
       </c>
       <c r="J38" s="91" t="s">
@@ -4288,7 +4303,7 @@
       <c r="N39" s="45">
         <v>252</v>
       </c>
-      <c r="O39" s="98">
+      <c r="O39" s="99">
         <v>5000</v>
       </c>
       <c r="P39" s="28"/>
@@ -4332,7 +4347,7 @@
       <c r="N40" s="45">
         <v>282</v>
       </c>
-      <c r="O40" s="98">
+      <c r="O40" s="99">
         <v>5000</v>
       </c>
       <c r="P40" s="27"/>
@@ -4376,7 +4391,7 @@
       <c r="N41" s="45">
         <v>192</v>
       </c>
-      <c r="O41" s="98">
+      <c r="O41" s="99">
         <v>2000</v>
       </c>
       <c r="P41" s="27"/>
@@ -4420,7 +4435,7 @@
       <c r="N42" s="45">
         <v>207</v>
       </c>
-      <c r="O42" s="98">
+      <c r="O42" s="99">
         <v>4000</v>
       </c>
       <c r="P42" s="27"/>
@@ -4465,7 +4480,7 @@
       <c r="N43" s="45">
         <v>387</v>
       </c>
-      <c r="O43" s="98">
+      <c r="O43" s="99">
         <v>1000</v>
       </c>
       <c r="P43" s="27"/>
@@ -4507,7 +4522,7 @@
         <v>72</v>
       </c>
       <c r="N44" s="45"/>
-      <c r="O44" s="98"/>
+      <c r="O44" s="99"/>
       <c r="Q44" s="40" t="s">
         <v>42</v>
       </c>
@@ -4548,7 +4563,7 @@
       <c r="L45" s="27"/>
       <c r="M45" s="28"/>
       <c r="N45" s="45"/>
-      <c r="O45" s="98"/>
+      <c r="O45" s="99"/>
       <c r="Q45" s="40" t="s">
         <v>117</v>
       </c>
@@ -4587,7 +4602,7 @@
       </c>
       <c r="L46" s="27"/>
       <c r="N46" s="45"/>
-      <c r="O46" s="98"/>
+      <c r="O46" s="99"/>
       <c r="Q46" s="40" t="s">
         <v>115</v>
       </c>
@@ -4626,7 +4641,7 @@
       </c>
       <c r="L47" s="27"/>
       <c r="N47" s="45"/>
-      <c r="O47" s="98"/>
+      <c r="O47" s="99"/>
       <c r="Q47" s="40" t="s">
         <v>116</v>
       </c>
@@ -4666,7 +4681,7 @@
       <c r="L48" s="28"/>
       <c r="M48" s="28"/>
       <c r="N48" s="45"/>
-      <c r="O48" s="98"/>
+      <c r="O48" s="99"/>
       <c r="Q48" s="40" t="s">
         <v>41</v>
       </c>
@@ -4706,7 +4721,7 @@
       </c>
       <c r="L49" s="28"/>
       <c r="N49" s="45"/>
-      <c r="O49" s="98"/>
+      <c r="O49" s="99"/>
       <c r="Q49" s="40" t="s">
         <v>41</v>
       </c>
@@ -4747,7 +4762,7 @@
       <c r="L50" s="28"/>
       <c r="M50" s="28"/>
       <c r="N50" s="45"/>
-      <c r="O50" s="98"/>
+      <c r="O50" s="99"/>
       <c r="Q50" s="40" t="s">
         <v>41</v>
       </c>
@@ -4787,7 +4802,7 @@
       </c>
       <c r="M51" s="27"/>
       <c r="N51" s="45"/>
-      <c r="O51" s="98"/>
+      <c r="O51" s="99"/>
       <c r="Q51" s="39">
         <v>8480011000022</v>
       </c>
@@ -4827,7 +4842,7 @@
       </c>
       <c r="M52" s="27"/>
       <c r="N52" s="45"/>
-      <c r="O52" s="98"/>
+      <c r="O52" s="99"/>
       <c r="Q52" s="39">
         <v>8480011000022</v>
       </c>
@@ -4867,7 +4882,7 @@
       </c>
       <c r="M53" s="27"/>
       <c r="N53" s="46"/>
-      <c r="O53" s="99"/>
+      <c r="O53" s="100"/>
       <c r="Q53" s="39" t="s">
         <v>44</v>
       </c>
@@ -4910,7 +4925,7 @@
       </c>
       <c r="S54" s="37"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="62">
         <v>280</v>
       </c>
@@ -4944,7 +4959,7 @@
       </c>
       <c r="S55" s="37"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="62">
         <v>290</v>
       </c>
@@ -4967,7 +4982,10 @@
       <c r="H56" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="N56" s="36"/>
+      <c r="N56" s="97" t="s">
+        <v>147</v>
+      </c>
+      <c r="O56" s="98"/>
       <c r="Q56" s="39" t="s">
         <v>26</v>
       </c>
@@ -4999,7 +5017,12 @@
       <c r="H57" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="N57" s="37"/>
+      <c r="N57" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="O57" s="38" t="s">
+        <v>6</v>
+      </c>
       <c r="Q57" s="39" t="s">
         <v>26</v>
       </c>
@@ -5032,7 +5055,8 @@
         <v>27</v>
       </c>
       <c r="L58" s="28"/>
-      <c r="N58" s="37"/>
+      <c r="N58" s="103"/>
+      <c r="O58" s="104"/>
       <c r="Q58" s="42" t="s">
         <v>26</v>
       </c>
@@ -5064,7 +5088,8 @@
       <c r="H59" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="N59" s="36"/>
+      <c r="N59" s="96"/>
+      <c r="O59" s="104"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="62">
@@ -5090,7 +5115,8 @@
         <v>27</v>
       </c>
       <c r="L60" s="28"/>
-      <c r="N60" s="37"/>
+      <c r="N60" s="103"/>
+      <c r="O60" s="104"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="62">
@@ -5116,7 +5142,8 @@
         <v>27</v>
       </c>
       <c r="L61" s="27"/>
-      <c r="N61" s="36"/>
+      <c r="N61" s="96"/>
+      <c r="O61" s="104"/>
     </row>
     <row r="62" spans="1:19" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="69">
@@ -5142,15 +5169,18 @@
         <v>27</v>
       </c>
       <c r="L62" s="27"/>
-      <c r="N62" s="27"/>
+      <c r="N62" s="96"/>
+      <c r="O62" s="104"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="L63" s="27"/>
-      <c r="N63" s="27"/>
+      <c r="N63" s="96"/>
+      <c r="O63" s="104"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="L64" s="27"/>
-      <c r="N64" s="27"/>
+      <c r="N64" s="96"/>
+      <c r="O64" s="104"/>
     </row>
     <row r="65" spans="6:18" x14ac:dyDescent="0.2">
       <c r="F65" s="24"/>
@@ -5158,7 +5188,8 @@
       <c r="H65" s="23"/>
       <c r="I65" s="23"/>
       <c r="J65" s="27"/>
-      <c r="N65" s="14"/>
+      <c r="N65" s="39"/>
+      <c r="O65" s="104"/>
       <c r="R65" s="23"/>
     </row>
     <row r="66" spans="6:18" x14ac:dyDescent="0.2">
@@ -5167,7 +5198,8 @@
       <c r="H66" s="23"/>
       <c r="I66" s="23"/>
       <c r="J66" s="23"/>
-      <c r="N66" s="14"/>
+      <c r="N66" s="39"/>
+      <c r="O66" s="104"/>
       <c r="R66" s="23"/>
     </row>
     <row r="67" spans="6:18" x14ac:dyDescent="0.2">
@@ -5176,7 +5208,8 @@
       <c r="H67" s="23"/>
       <c r="I67" s="23"/>
       <c r="J67" s="23"/>
-      <c r="N67" s="14"/>
+      <c r="N67" s="39"/>
+      <c r="O67" s="104"/>
       <c r="R67" s="23"/>
     </row>
     <row r="68" spans="6:18" x14ac:dyDescent="0.2">
@@ -5185,7 +5218,8 @@
       <c r="H68" s="23"/>
       <c r="I68" s="23"/>
       <c r="J68" s="23"/>
-      <c r="N68" s="14"/>
+      <c r="N68" s="39"/>
+      <c r="O68" s="104"/>
       <c r="R68" s="23"/>
     </row>
     <row r="69" spans="6:18" x14ac:dyDescent="0.2">
@@ -5194,16 +5228,18 @@
       <c r="H69" s="23"/>
       <c r="I69" s="23"/>
       <c r="J69" s="23"/>
-      <c r="N69" s="14"/>
+      <c r="N69" s="39"/>
+      <c r="O69" s="104"/>
       <c r="R69" s="23"/>
     </row>
-    <row r="70" spans="6:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="6:18" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F70" s="24"/>
       <c r="G70" s="23"/>
       <c r="H70" s="23"/>
       <c r="I70" s="23"/>
       <c r="J70" s="23"/>
-      <c r="N70" s="14"/>
+      <c r="N70" s="42"/>
+      <c r="O70" s="105"/>
       <c r="R70" s="23"/>
     </row>
     <row r="71" spans="6:18" x14ac:dyDescent="0.2">
@@ -5408,7 +5444,8 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J39:K53">
     <sortCondition ref="K39:K53"/>
   </sortState>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="N56:O56"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="A3:G3"/>

</xml_diff>